<commit_message>
Committing all deleted files
</commit_message>
<xml_diff>
--- a/sectors.xlsx
+++ b/sectors.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="907">
   <si>
     <t xml:space="preserve">ticker</t>
   </si>
@@ -2556,6 +2556,183 @@
   </si>
   <si>
     <t xml:space="preserve">ZIGNAGO VETRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTILIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERVIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FINANC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CYCLIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AEROPORTO G MARCONI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALERION CLEANPOWER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TECHNO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEALTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPGDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BASICM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AZIMUT HOLDING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BANCA PROFILO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BASTOGI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NONCYC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BP SONDRIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUZZI UNICEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAREL INDUSTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEMENTIR HOLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CENTRALE LATTE IT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIVITANAVI SYS N-S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMER INDUSTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMPAGNIA IMM AZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREDITO EMILIANO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSP INTERNATIONAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAMICO INTERNATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE LONGHI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIGIT VAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E.P.H.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EL.EN.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EUROGRP LAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FINE FOODS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GABETTI PROPERTY SOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAROFALO H CARE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GENERALI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IGD.MI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IGD SIIQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN DE NORA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT EXHIBIT GRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IVECO GRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAZIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOTTOMATICA GR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LU-VE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFEB.MI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFE-MEDIA RG-B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONDADORI EDITORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NETWEEK RAGGR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIAGGIO &amp; C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PININFARINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIRELLI &amp; C.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECORDATI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STMMI.MI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STMICROELECTRONICS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAMBURI INC PARTN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TECHNOPR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THE IT SEA GRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TREVI FINAN IND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TXT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VINCENZO ZUCCHI</t>
   </si>
 </sst>
 </file>
@@ -7441,6 +7618,2206 @@
         <v>105</v>
       </c>
     </row>
+    <row r="415">
+      <c r="A415" t="s">
+        <v>3</v>
+      </c>
+      <c r="B415" t="s">
+        <v>4</v>
+      </c>
+      <c r="C415" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="s">
+        <v>15</v>
+      </c>
+      <c r="B416" t="s">
+        <v>16</v>
+      </c>
+      <c r="C416" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="s">
+        <v>22</v>
+      </c>
+      <c r="B417" t="s">
+        <v>23</v>
+      </c>
+      <c r="C417" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="s">
+        <v>30</v>
+      </c>
+      <c r="B418" t="s">
+        <v>31</v>
+      </c>
+      <c r="C418" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="s">
+        <v>32</v>
+      </c>
+      <c r="B419" t="s">
+        <v>33</v>
+      </c>
+      <c r="C419" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="s">
+        <v>27</v>
+      </c>
+      <c r="B420" t="s">
+        <v>852</v>
+      </c>
+      <c r="C420" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="s">
+        <v>64</v>
+      </c>
+      <c r="B421" t="s">
+        <v>854</v>
+      </c>
+      <c r="C421" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="s">
+        <v>49</v>
+      </c>
+      <c r="B422" t="s">
+        <v>50</v>
+      </c>
+      <c r="C422" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="s">
+        <v>47</v>
+      </c>
+      <c r="B423" t="s">
+        <v>48</v>
+      </c>
+      <c r="C423" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="s">
+        <v>53</v>
+      </c>
+      <c r="B424" t="s">
+        <v>54</v>
+      </c>
+      <c r="C424" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="s">
+        <v>56</v>
+      </c>
+      <c r="B425" t="s">
+        <v>57</v>
+      </c>
+      <c r="C425" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="s">
+        <v>75</v>
+      </c>
+      <c r="B426" t="s">
+        <v>76</v>
+      </c>
+      <c r="C426" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="s">
+        <v>250</v>
+      </c>
+      <c r="B427" t="s">
+        <v>251</v>
+      </c>
+      <c r="C427" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="s">
+        <v>69</v>
+      </c>
+      <c r="B428" t="s">
+        <v>70</v>
+      </c>
+      <c r="C428" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="s">
+        <v>78</v>
+      </c>
+      <c r="B429" t="s">
+        <v>79</v>
+      </c>
+      <c r="C429" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="s">
+        <v>80</v>
+      </c>
+      <c r="B430" t="s">
+        <v>859</v>
+      </c>
+      <c r="C430" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="s">
+        <v>94</v>
+      </c>
+      <c r="B431" t="s">
+        <v>95</v>
+      </c>
+      <c r="C431" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="s">
+        <v>106</v>
+      </c>
+      <c r="B432" t="s">
+        <v>107</v>
+      </c>
+      <c r="C432" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="s">
+        <v>422</v>
+      </c>
+      <c r="B433" t="s">
+        <v>423</v>
+      </c>
+      <c r="C433" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="s">
+        <v>114</v>
+      </c>
+      <c r="B434" t="s">
+        <v>115</v>
+      </c>
+      <c r="C434" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="s">
+        <v>614</v>
+      </c>
+      <c r="B435" t="s">
+        <v>860</v>
+      </c>
+      <c r="C435" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="s">
+        <v>130</v>
+      </c>
+      <c r="B436" t="s">
+        <v>131</v>
+      </c>
+      <c r="C436" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="s">
+        <v>84</v>
+      </c>
+      <c r="B437" t="s">
+        <v>85</v>
+      </c>
+      <c r="C437" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="s">
+        <v>86</v>
+      </c>
+      <c r="B438" t="s">
+        <v>87</v>
+      </c>
+      <c r="C438" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="s">
+        <v>82</v>
+      </c>
+      <c r="B439" t="s">
+        <v>861</v>
+      </c>
+      <c r="C439" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="s">
+        <v>132</v>
+      </c>
+      <c r="B440" t="s">
+        <v>133</v>
+      </c>
+      <c r="C440" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="s">
+        <v>92</v>
+      </c>
+      <c r="B441" t="s">
+        <v>93</v>
+      </c>
+      <c r="C441" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="s">
+        <v>99</v>
+      </c>
+      <c r="B442" t="s">
+        <v>100</v>
+      </c>
+      <c r="C442" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="s">
+        <v>101</v>
+      </c>
+      <c r="B443" t="s">
+        <v>102</v>
+      </c>
+      <c r="C443" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="s">
+        <v>108</v>
+      </c>
+      <c r="B444" t="s">
+        <v>109</v>
+      </c>
+      <c r="C444" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="s">
+        <v>128</v>
+      </c>
+      <c r="B445" t="s">
+        <v>129</v>
+      </c>
+      <c r="C445" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="s">
+        <v>110</v>
+      </c>
+      <c r="B446" t="s">
+        <v>111</v>
+      </c>
+      <c r="C446" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="s">
+        <v>118</v>
+      </c>
+      <c r="B447" t="s">
+        <v>119</v>
+      </c>
+      <c r="C447" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="s">
+        <v>122</v>
+      </c>
+      <c r="B448" t="s">
+        <v>863</v>
+      </c>
+      <c r="C448" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="s">
+        <v>120</v>
+      </c>
+      <c r="B449" t="s">
+        <v>121</v>
+      </c>
+      <c r="C449" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="s">
+        <v>124</v>
+      </c>
+      <c r="B450" t="s">
+        <v>125</v>
+      </c>
+      <c r="C450" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="s">
+        <v>126</v>
+      </c>
+      <c r="B451" t="s">
+        <v>127</v>
+      </c>
+      <c r="C451" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="s">
+        <v>88</v>
+      </c>
+      <c r="B452" t="s">
+        <v>89</v>
+      </c>
+      <c r="C452" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="s">
+        <v>134</v>
+      </c>
+      <c r="B453" t="s">
+        <v>864</v>
+      </c>
+      <c r="C453" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="s">
+        <v>137</v>
+      </c>
+      <c r="B454" t="s">
+        <v>138</v>
+      </c>
+      <c r="C454" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="s">
+        <v>169</v>
+      </c>
+      <c r="B455" t="s">
+        <v>170</v>
+      </c>
+      <c r="C455" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="s">
+        <v>139</v>
+      </c>
+      <c r="B456" t="s">
+        <v>140</v>
+      </c>
+      <c r="C456" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="s">
+        <v>189</v>
+      </c>
+      <c r="B457" t="s">
+        <v>190</v>
+      </c>
+      <c r="C457" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="s">
+        <v>191</v>
+      </c>
+      <c r="B458" t="s">
+        <v>865</v>
+      </c>
+      <c r="C458" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="s">
+        <v>149</v>
+      </c>
+      <c r="B459" t="s">
+        <v>150</v>
+      </c>
+      <c r="C459" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="s">
+        <v>173</v>
+      </c>
+      <c r="B460" t="s">
+        <v>174</v>
+      </c>
+      <c r="C460" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="s">
+        <v>151</v>
+      </c>
+      <c r="B461" t="s">
+        <v>866</v>
+      </c>
+      <c r="C461" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="s">
+        <v>171</v>
+      </c>
+      <c r="B462" t="s">
+        <v>867</v>
+      </c>
+      <c r="C462" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="s">
+        <v>161</v>
+      </c>
+      <c r="B463" t="s">
+        <v>162</v>
+      </c>
+      <c r="C463" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="s">
+        <v>179</v>
+      </c>
+      <c r="B464" t="s">
+        <v>868</v>
+      </c>
+      <c r="C464" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="s">
+        <v>167</v>
+      </c>
+      <c r="B465" t="s">
+        <v>168</v>
+      </c>
+      <c r="C465" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="s">
+        <v>181</v>
+      </c>
+      <c r="B466" t="s">
+        <v>869</v>
+      </c>
+      <c r="C466" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="s">
+        <v>159</v>
+      </c>
+      <c r="B467" t="s">
+        <v>870</v>
+      </c>
+      <c r="C467" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="s">
+        <v>177</v>
+      </c>
+      <c r="B468" t="s">
+        <v>178</v>
+      </c>
+      <c r="C468" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="s">
+        <v>145</v>
+      </c>
+      <c r="B469" t="s">
+        <v>871</v>
+      </c>
+      <c r="C469" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="s">
+        <v>193</v>
+      </c>
+      <c r="B470" t="s">
+        <v>872</v>
+      </c>
+      <c r="C470" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="s">
+        <v>202</v>
+      </c>
+      <c r="B471" t="s">
+        <v>203</v>
+      </c>
+      <c r="C471" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="s">
+        <v>228</v>
+      </c>
+      <c r="B472" t="s">
+        <v>873</v>
+      </c>
+      <c r="C472" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="s">
+        <v>210</v>
+      </c>
+      <c r="B473" t="s">
+        <v>211</v>
+      </c>
+      <c r="C473" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="s">
+        <v>208</v>
+      </c>
+      <c r="B474" t="s">
+        <v>209</v>
+      </c>
+      <c r="C474" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="s">
+        <v>232</v>
+      </c>
+      <c r="B475" t="s">
+        <v>874</v>
+      </c>
+      <c r="C475" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="s">
+        <v>216</v>
+      </c>
+      <c r="B476" t="s">
+        <v>217</v>
+      </c>
+      <c r="C476" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="s">
+        <v>224</v>
+      </c>
+      <c r="B477" t="s">
+        <v>225</v>
+      </c>
+      <c r="C477" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="s">
+        <v>220</v>
+      </c>
+      <c r="B478" t="s">
+        <v>875</v>
+      </c>
+      <c r="C478" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="s">
+        <v>226</v>
+      </c>
+      <c r="B479" t="s">
+        <v>227</v>
+      </c>
+      <c r="C479" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="s">
+        <v>238</v>
+      </c>
+      <c r="B480" t="s">
+        <v>239</v>
+      </c>
+      <c r="C480" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="s">
+        <v>285</v>
+      </c>
+      <c r="B481" t="s">
+        <v>876</v>
+      </c>
+      <c r="C481" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="s">
+        <v>256</v>
+      </c>
+      <c r="B482" t="s">
+        <v>257</v>
+      </c>
+      <c r="C482" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="s">
+        <v>268</v>
+      </c>
+      <c r="B483" t="s">
+        <v>877</v>
+      </c>
+      <c r="C483" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="s">
+        <v>264</v>
+      </c>
+      <c r="B484" t="s">
+        <v>265</v>
+      </c>
+      <c r="C484" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="s">
+        <v>272</v>
+      </c>
+      <c r="B485" t="s">
+        <v>273</v>
+      </c>
+      <c r="C485" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="s">
+        <v>274</v>
+      </c>
+      <c r="B486" t="s">
+        <v>275</v>
+      </c>
+      <c r="C486" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="s">
+        <v>276</v>
+      </c>
+      <c r="B487" t="s">
+        <v>277</v>
+      </c>
+      <c r="C487" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="s">
+        <v>281</v>
+      </c>
+      <c r="B488" t="s">
+        <v>282</v>
+      </c>
+      <c r="C488" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="s">
+        <v>278</v>
+      </c>
+      <c r="B489" t="s">
+        <v>279</v>
+      </c>
+      <c r="C489" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="s">
+        <v>289</v>
+      </c>
+      <c r="B490" t="s">
+        <v>290</v>
+      </c>
+      <c r="C490" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="s">
+        <v>293</v>
+      </c>
+      <c r="B491" t="s">
+        <v>294</v>
+      </c>
+      <c r="C491" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="s">
+        <v>616</v>
+      </c>
+      <c r="B492" t="s">
+        <v>617</v>
+      </c>
+      <c r="C492" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="s">
+        <v>260</v>
+      </c>
+      <c r="B493" t="s">
+        <v>878</v>
+      </c>
+      <c r="C493" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="s">
+        <v>303</v>
+      </c>
+      <c r="B494" t="s">
+        <v>304</v>
+      </c>
+      <c r="C494" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="s">
+        <v>832</v>
+      </c>
+      <c r="B495" t="s">
+        <v>833</v>
+      </c>
+      <c r="C495" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="s">
+        <v>630</v>
+      </c>
+      <c r="B496" t="s">
+        <v>631</v>
+      </c>
+      <c r="C496" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="s">
+        <v>834</v>
+      </c>
+      <c r="B497" t="s">
+        <v>835</v>
+      </c>
+      <c r="C497" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="s">
+        <v>328</v>
+      </c>
+      <c r="B498" t="s">
+        <v>329</v>
+      </c>
+      <c r="C498" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="s">
+        <v>338</v>
+      </c>
+      <c r="B499" t="s">
+        <v>339</v>
+      </c>
+      <c r="C499" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="s">
+        <v>334</v>
+      </c>
+      <c r="B500" t="s">
+        <v>335</v>
+      </c>
+      <c r="C500" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="s">
+        <v>326</v>
+      </c>
+      <c r="B501" t="s">
+        <v>327</v>
+      </c>
+      <c r="C501" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="s">
+        <v>330</v>
+      </c>
+      <c r="B502" t="s">
+        <v>879</v>
+      </c>
+      <c r="C502" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="s">
+        <v>320</v>
+      </c>
+      <c r="B503" t="s">
+        <v>321</v>
+      </c>
+      <c r="C503" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="s">
+        <v>340</v>
+      </c>
+      <c r="B504" t="s">
+        <v>341</v>
+      </c>
+      <c r="C504" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="s">
+        <v>358</v>
+      </c>
+      <c r="B505" t="s">
+        <v>880</v>
+      </c>
+      <c r="C505" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="s">
+        <v>376</v>
+      </c>
+      <c r="B506" t="s">
+        <v>881</v>
+      </c>
+      <c r="C506" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="s">
+        <v>394</v>
+      </c>
+      <c r="B507" t="s">
+        <v>395</v>
+      </c>
+      <c r="C507" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="s">
+        <v>366</v>
+      </c>
+      <c r="B508" t="s">
+        <v>367</v>
+      </c>
+      <c r="C508" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="s">
+        <v>356</v>
+      </c>
+      <c r="B509" t="s">
+        <v>882</v>
+      </c>
+      <c r="C509" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="s">
+        <v>370</v>
+      </c>
+      <c r="B510" t="s">
+        <v>371</v>
+      </c>
+      <c r="C510" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="s">
+        <v>374</v>
+      </c>
+      <c r="B511" t="s">
+        <v>375</v>
+      </c>
+      <c r="C511" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="s">
+        <v>386</v>
+      </c>
+      <c r="B512" t="s">
+        <v>387</v>
+      </c>
+      <c r="C512" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="s">
+        <v>398</v>
+      </c>
+      <c r="B513" t="s">
+        <v>399</v>
+      </c>
+      <c r="C513" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="s">
+        <v>400</v>
+      </c>
+      <c r="B514" t="s">
+        <v>401</v>
+      </c>
+      <c r="C514" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="s">
+        <v>402</v>
+      </c>
+      <c r="B515" t="s">
+        <v>403</v>
+      </c>
+      <c r="C515" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="s">
+        <v>426</v>
+      </c>
+      <c r="B516" t="s">
+        <v>427</v>
+      </c>
+      <c r="C516" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="s">
+        <v>883</v>
+      </c>
+      <c r="B517" t="s">
+        <v>884</v>
+      </c>
+      <c r="C517" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="s">
+        <v>668</v>
+      </c>
+      <c r="B518" t="s">
+        <v>669</v>
+      </c>
+      <c r="C518" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="s">
+        <v>434</v>
+      </c>
+      <c r="B519" t="s">
+        <v>435</v>
+      </c>
+      <c r="C519" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="s">
+        <v>440</v>
+      </c>
+      <c r="B520" t="s">
+        <v>441</v>
+      </c>
+      <c r="C520" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="s">
+        <v>234</v>
+      </c>
+      <c r="B521" t="s">
+        <v>885</v>
+      </c>
+      <c r="C521" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="s">
+        <v>414</v>
+      </c>
+      <c r="B522" t="s">
+        <v>415</v>
+      </c>
+      <c r="C522" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="s">
+        <v>452</v>
+      </c>
+      <c r="B523" t="s">
+        <v>453</v>
+      </c>
+      <c r="C523" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="s">
+        <v>460</v>
+      </c>
+      <c r="B524" t="s">
+        <v>461</v>
+      </c>
+      <c r="C524" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="s">
+        <v>448</v>
+      </c>
+      <c r="B525" t="s">
+        <v>449</v>
+      </c>
+      <c r="C525" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="s">
+        <v>454</v>
+      </c>
+      <c r="B526" t="s">
+        <v>455</v>
+      </c>
+      <c r="C526" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="s">
+        <v>456</v>
+      </c>
+      <c r="B527" t="s">
+        <v>457</v>
+      </c>
+      <c r="C527" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="s">
+        <v>420</v>
+      </c>
+      <c r="B528" t="s">
+        <v>886</v>
+      </c>
+      <c r="C528" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="s">
+        <v>466</v>
+      </c>
+      <c r="B529" t="s">
+        <v>467</v>
+      </c>
+      <c r="C529" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="s">
+        <v>424</v>
+      </c>
+      <c r="B530" t="s">
+        <v>425</v>
+      </c>
+      <c r="C530" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="s">
+        <v>464</v>
+      </c>
+      <c r="B531" t="s">
+        <v>465</v>
+      </c>
+      <c r="C531" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="s">
+        <v>468</v>
+      </c>
+      <c r="B532" t="s">
+        <v>887</v>
+      </c>
+      <c r="C532" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="s">
+        <v>472</v>
+      </c>
+      <c r="B533" t="s">
+        <v>473</v>
+      </c>
+      <c r="C533" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="s">
+        <v>478</v>
+      </c>
+      <c r="B534" t="s">
+        <v>479</v>
+      </c>
+      <c r="C534" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="s">
+        <v>482</v>
+      </c>
+      <c r="B535" t="s">
+        <v>483</v>
+      </c>
+      <c r="C535" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="s">
+        <v>494</v>
+      </c>
+      <c r="B536" t="s">
+        <v>495</v>
+      </c>
+      <c r="C536" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="s">
+        <v>730</v>
+      </c>
+      <c r="B537" t="s">
+        <v>888</v>
+      </c>
+      <c r="C537" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="s">
+        <v>488</v>
+      </c>
+      <c r="B538" t="s">
+        <v>489</v>
+      </c>
+      <c r="C538" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="s">
+        <v>500</v>
+      </c>
+      <c r="B539" t="s">
+        <v>889</v>
+      </c>
+      <c r="C539" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="s">
+        <v>502</v>
+      </c>
+      <c r="B540" t="s">
+        <v>890</v>
+      </c>
+      <c r="C540" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="s">
+        <v>504</v>
+      </c>
+      <c r="B541" t="s">
+        <v>505</v>
+      </c>
+      <c r="C541" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="s">
+        <v>510</v>
+      </c>
+      <c r="B542" t="s">
+        <v>511</v>
+      </c>
+      <c r="C542" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="s">
+        <v>514</v>
+      </c>
+      <c r="B543" t="s">
+        <v>515</v>
+      </c>
+      <c r="C543" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="s">
+        <v>518</v>
+      </c>
+      <c r="B544" t="s">
+        <v>519</v>
+      </c>
+      <c r="C544" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="s">
+        <v>891</v>
+      </c>
+      <c r="B545" t="s">
+        <v>892</v>
+      </c>
+      <c r="C545" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="s">
+        <v>538</v>
+      </c>
+      <c r="B546" t="s">
+        <v>539</v>
+      </c>
+      <c r="C546" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="s">
+        <v>530</v>
+      </c>
+      <c r="B547" t="s">
+        <v>893</v>
+      </c>
+      <c r="C547" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="s">
+        <v>546</v>
+      </c>
+      <c r="B548" t="s">
+        <v>547</v>
+      </c>
+      <c r="C548" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="s">
+        <v>536</v>
+      </c>
+      <c r="B549" t="s">
+        <v>537</v>
+      </c>
+      <c r="C549" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="s">
+        <v>534</v>
+      </c>
+      <c r="B550" t="s">
+        <v>535</v>
+      </c>
+      <c r="C550" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="s">
+        <v>550</v>
+      </c>
+      <c r="B551" t="s">
+        <v>551</v>
+      </c>
+      <c r="C551" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="s">
+        <v>560</v>
+      </c>
+      <c r="B552" t="s">
+        <v>894</v>
+      </c>
+      <c r="C552" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="s">
+        <v>566</v>
+      </c>
+      <c r="B553" t="s">
+        <v>567</v>
+      </c>
+      <c r="C553" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="s">
+        <v>552</v>
+      </c>
+      <c r="B554" t="s">
+        <v>553</v>
+      </c>
+      <c r="C554" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="s">
+        <v>570</v>
+      </c>
+      <c r="B555" t="s">
+        <v>571</v>
+      </c>
+      <c r="C555" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="s">
+        <v>568</v>
+      </c>
+      <c r="B556" t="s">
+        <v>569</v>
+      </c>
+      <c r="C556" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="s">
+        <v>574</v>
+      </c>
+      <c r="B557" t="s">
+        <v>575</v>
+      </c>
+      <c r="C557" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="s">
+        <v>580</v>
+      </c>
+      <c r="B558" t="s">
+        <v>581</v>
+      </c>
+      <c r="C558" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="s">
+        <v>590</v>
+      </c>
+      <c r="B559" t="s">
+        <v>591</v>
+      </c>
+      <c r="C559" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="s">
+        <v>588</v>
+      </c>
+      <c r="B560" t="s">
+        <v>589</v>
+      </c>
+      <c r="C560" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="s">
+        <v>592</v>
+      </c>
+      <c r="B561" t="s">
+        <v>895</v>
+      </c>
+      <c r="C561" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="s">
+        <v>594</v>
+      </c>
+      <c r="B562" t="s">
+        <v>896</v>
+      </c>
+      <c r="C562" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="s">
+        <v>626</v>
+      </c>
+      <c r="B563" t="s">
+        <v>627</v>
+      </c>
+      <c r="C563" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="s">
+        <v>610</v>
+      </c>
+      <c r="B564" t="s">
+        <v>611</v>
+      </c>
+      <c r="C564" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="s">
+        <v>596</v>
+      </c>
+      <c r="B565" t="s">
+        <v>897</v>
+      </c>
+      <c r="C565" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="s">
+        <v>598</v>
+      </c>
+      <c r="B566" t="s">
+        <v>599</v>
+      </c>
+      <c r="C566" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="s">
+        <v>622</v>
+      </c>
+      <c r="B567" t="s">
+        <v>623</v>
+      </c>
+      <c r="C567" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="s">
+        <v>618</v>
+      </c>
+      <c r="B568" t="s">
+        <v>619</v>
+      </c>
+      <c r="C568" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="s">
+        <v>664</v>
+      </c>
+      <c r="B569" t="s">
+        <v>665</v>
+      </c>
+      <c r="C569" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="s">
+        <v>636</v>
+      </c>
+      <c r="B570" t="s">
+        <v>637</v>
+      </c>
+      <c r="C570" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="s">
+        <v>642</v>
+      </c>
+      <c r="B571" t="s">
+        <v>898</v>
+      </c>
+      <c r="C571" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="s">
+        <v>650</v>
+      </c>
+      <c r="B572" t="s">
+        <v>651</v>
+      </c>
+      <c r="C572" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="s">
+        <v>662</v>
+      </c>
+      <c r="B573" t="s">
+        <v>663</v>
+      </c>
+      <c r="C573" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="s">
+        <v>672</v>
+      </c>
+      <c r="B574" t="s">
+        <v>673</v>
+      </c>
+      <c r="C574" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="s">
+        <v>696</v>
+      </c>
+      <c r="B575" t="s">
+        <v>697</v>
+      </c>
+      <c r="C575" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="s">
+        <v>692</v>
+      </c>
+      <c r="B576" t="s">
+        <v>693</v>
+      </c>
+      <c r="C576" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="s">
+        <v>720</v>
+      </c>
+      <c r="B577" t="s">
+        <v>721</v>
+      </c>
+      <c r="C577" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="s">
+        <v>678</v>
+      </c>
+      <c r="B578" t="s">
+        <v>679</v>
+      </c>
+      <c r="C578" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="s">
+        <v>690</v>
+      </c>
+      <c r="B579" t="s">
+        <v>691</v>
+      </c>
+      <c r="C579" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="s">
+        <v>710</v>
+      </c>
+      <c r="B580" t="s">
+        <v>711</v>
+      </c>
+      <c r="C580" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="s">
+        <v>728</v>
+      </c>
+      <c r="B581" t="s">
+        <v>729</v>
+      </c>
+      <c r="C581" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="s">
+        <v>450</v>
+      </c>
+      <c r="B582" t="s">
+        <v>451</v>
+      </c>
+      <c r="C582" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="s">
+        <v>686</v>
+      </c>
+      <c r="B583" t="s">
+        <v>687</v>
+      </c>
+      <c r="C583" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="s">
+        <v>726</v>
+      </c>
+      <c r="B584" t="s">
+        <v>727</v>
+      </c>
+      <c r="C584" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="s">
+        <v>688</v>
+      </c>
+      <c r="B585" t="s">
+        <v>689</v>
+      </c>
+      <c r="C585" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="s">
+        <v>708</v>
+      </c>
+      <c r="B586" t="s">
+        <v>709</v>
+      </c>
+      <c r="C586" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="s">
+        <v>724</v>
+      </c>
+      <c r="B587" t="s">
+        <v>725</v>
+      </c>
+      <c r="C587" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="s">
+        <v>694</v>
+      </c>
+      <c r="B588" t="s">
+        <v>695</v>
+      </c>
+      <c r="C588" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="s">
+        <v>700</v>
+      </c>
+      <c r="B589" t="s">
+        <v>701</v>
+      </c>
+      <c r="C589" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="s">
+        <v>714</v>
+      </c>
+      <c r="B590" t="s">
+        <v>715</v>
+      </c>
+      <c r="C590" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="s">
+        <v>716</v>
+      </c>
+      <c r="B591" t="s">
+        <v>717</v>
+      </c>
+      <c r="C591" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="s">
+        <v>899</v>
+      </c>
+      <c r="B592" t="s">
+        <v>900</v>
+      </c>
+      <c r="C592" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="s">
+        <v>756</v>
+      </c>
+      <c r="B593" t="s">
+        <v>901</v>
+      </c>
+      <c r="C593" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="s">
+        <v>752</v>
+      </c>
+      <c r="B594" t="s">
+        <v>753</v>
+      </c>
+      <c r="C594" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="s">
+        <v>774</v>
+      </c>
+      <c r="B595" t="s">
+        <v>902</v>
+      </c>
+      <c r="C595" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="s">
+        <v>760</v>
+      </c>
+      <c r="B596" t="s">
+        <v>761</v>
+      </c>
+      <c r="C596" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="s">
+        <v>746</v>
+      </c>
+      <c r="B597" t="s">
+        <v>747</v>
+      </c>
+      <c r="C597" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="s">
+        <v>780</v>
+      </c>
+      <c r="B598" t="s">
+        <v>781</v>
+      </c>
+      <c r="C598" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="s">
+        <v>748</v>
+      </c>
+      <c r="B599" t="s">
+        <v>749</v>
+      </c>
+      <c r="C599" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="s">
+        <v>782</v>
+      </c>
+      <c r="B600" t="s">
+        <v>783</v>
+      </c>
+      <c r="C600" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="s">
+        <v>758</v>
+      </c>
+      <c r="B601" t="s">
+        <v>903</v>
+      </c>
+      <c r="C601" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="s">
+        <v>770</v>
+      </c>
+      <c r="B602" t="s">
+        <v>771</v>
+      </c>
+      <c r="C602" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="s">
+        <v>750</v>
+      </c>
+      <c r="B603" t="s">
+        <v>904</v>
+      </c>
+      <c r="C603" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="s">
+        <v>740</v>
+      </c>
+      <c r="B604" t="s">
+        <v>741</v>
+      </c>
+      <c r="C604" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="s">
+        <v>788</v>
+      </c>
+      <c r="B605" t="s">
+        <v>905</v>
+      </c>
+      <c r="C605" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="s">
+        <v>796</v>
+      </c>
+      <c r="B606" t="s">
+        <v>797</v>
+      </c>
+      <c r="C606" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="s">
+        <v>798</v>
+      </c>
+      <c r="B607" t="s">
+        <v>799</v>
+      </c>
+      <c r="C607" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="s">
+        <v>802</v>
+      </c>
+      <c r="B608" t="s">
+        <v>803</v>
+      </c>
+      <c r="C608" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="s">
+        <v>800</v>
+      </c>
+      <c r="B609" t="s">
+        <v>801</v>
+      </c>
+      <c r="C609" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="s">
+        <v>816</v>
+      </c>
+      <c r="B610" t="s">
+        <v>817</v>
+      </c>
+      <c r="C610" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="s">
+        <v>844</v>
+      </c>
+      <c r="B611" t="s">
+        <v>906</v>
+      </c>
+      <c r="C611" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="s">
+        <v>824</v>
+      </c>
+      <c r="B612" t="s">
+        <v>825</v>
+      </c>
+      <c r="C612" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="s">
+        <v>828</v>
+      </c>
+      <c r="B613" t="s">
+        <v>829</v>
+      </c>
+      <c r="C613" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="s">
+        <v>846</v>
+      </c>
+      <c r="B614" t="s">
+        <v>847</v>
+      </c>
+      <c r="C614" t="s">
+        <v>858</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>